<commit_message>
implement junit report and change the config. Now only one sheet can be run which is config in the config file
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Environment</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -77,9 +77,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>Login Main Site</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -133,6 +130,16 @@
   </si>
   <si>
     <t>Test Result Folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Firefox</t>
+  </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>Test Suite</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -550,7 +557,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -594,10 +601,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -619,86 +626,98 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3"/>
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C10" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"Firefox, Chrome"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"Firefox, Chrome"</formula1>
+      <formula1>"Smoke, Function"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -707,10 +726,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -731,86 +750,98 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="3"/>
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="4">
         <v>2</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C10" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"Firefox, Chrome"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"Firefox, Chrome"</formula1>
+      <formula1>"Smoke, Function"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>